<commit_message>
finishing upload kontrak using job
</commit_message>
<xml_diff>
--- a/public/template/template_upload_kontrak.xlsx
+++ b/public/template/template_upload_kontrak.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\PROJECT TCF 202\tcf-superapps\public\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9ba44de7df4c40bc/Documents/HRIS - PT TRI CENTRUM FORTUNA/CODE/tcf-superapps/public/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{545BC130-A4FB-4FF5-BBFA-C70B407E8504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="13_ncr:1_{545BC130-A4FB-4FF5-BBFA-C70B407E8504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C235118C-18F2-4AE2-B135-FE62D02FCFDC}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9D850D6C-A414-4510-85CE-67383360A39D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{9D850D6C-A414-4510-85CE-67383360A39D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,69 +34,72 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
-  <si>
-    <t>Ex : FATHAN PEBRI (Gunakan Huruf Kapital)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Ex : 480.030524</t>
   </si>
   <si>
-    <t>Nama *</t>
-  </si>
-  <si>
-    <t>Nomor Induk Karyawan *</t>
-  </si>
-  <si>
-    <t>ID Posisi *</t>
-  </si>
-  <si>
     <t>Ambil data ini di Export Menu dan centang bagian Posisi</t>
   </si>
   <si>
-    <t>No Surat *</t>
-  </si>
-  <si>
     <t>Ex: No. 001/PKWT-I/HRD-TCF3/2024</t>
   </si>
   <si>
-    <t>Jenis Perjanjian Kerja *</t>
-  </si>
-  <si>
     <t>Ex : (PKWT, PKWTT, MAGANG)</t>
   </si>
   <si>
-    <t>Durasi (Bulan) *</t>
-  </si>
-  <si>
-    <t>Ex : 6</t>
-  </si>
-  <si>
-    <t>Tanggal Mulai *</t>
-  </si>
-  <si>
-    <t>Tanggal Selesai *</t>
-  </si>
-  <si>
     <t>Ex : 17/02/2024</t>
   </si>
   <si>
     <t>Ex : 17/08/2024</t>
   </si>
   <si>
-    <t>Salary *</t>
-  </si>
-  <si>
-    <t>Ex : 5250000</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Tempat Administrasi *</t>
-  </si>
-  <si>
-    <t>Ex : Karawang / Purwakarta (Sesuaikan dengan format ini)</t>
+    <t>Nomor Induk Karyawan (Database)</t>
+  </si>
+  <si>
+    <t>Nama (Free Text)</t>
+  </si>
+  <si>
+    <t>ID Posisi (Database)</t>
+  </si>
+  <si>
+    <t>Nama Posisi (Free Text)</t>
+  </si>
+  <si>
+    <t>Hanya untuk kebutuhan VLOOKUP</t>
+  </si>
+  <si>
+    <t>No Surat (Free Text)</t>
+  </si>
+  <si>
+    <t>Jenis Perjanjian Kerja (Option)</t>
+  </si>
+  <si>
+    <t>Durasi (Numeric)</t>
+  </si>
+  <si>
+    <t>Isi 0 untuk PKWTT</t>
+  </si>
+  <si>
+    <t>Salary (Numeric)</t>
+  </si>
+  <si>
+    <t>Isi tanpa tanda baca</t>
+  </si>
+  <si>
+    <t>Tanggal Mulai (dd/mm/yyyy)</t>
+  </si>
+  <si>
+    <t>Tanggal Selesai (dd/mm/yyyy)</t>
+  </si>
+  <si>
+    <t>Tempat Administrasi (Free Text)</t>
+  </si>
+  <si>
+    <t>Ex : Karawang</t>
   </si>
 </sst>
 </file>
@@ -118,7 +121,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -128,6 +131,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -170,10 +179,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -488,92 +498,100 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69D0E4EC-B375-444C-A099-75B908B6C530}">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="105" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.140625" customWidth="1"/>
-    <col min="3" max="3" width="51.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32" customWidth="1"/>
-    <col min="5" max="6" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.7109375" customWidth="1"/>
-    <col min="8" max="8" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="53" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.54296875" customWidth="1"/>
+    <col min="5" max="5" width="32" customWidth="1"/>
+    <col min="6" max="6" width="36.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.7265625" customWidth="1"/>
+    <col min="9" max="9" width="33" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="35.26953125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="53" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11" ht="17" x14ac:dyDescent="0.5">
+      <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="J2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I16" t="s">
         <v>6</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H16" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>